<commit_message>
add greed 376 402
</commit_message>
<xml_diff>
--- a/leetcode/leetcode.xlsx
+++ b/leetcode/leetcode.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workshop\git\Algorithm\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF254D8-9A1D-43C2-9D9F-5B83735CC88D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B1657B-6562-41D9-8EAA-2B923ED796A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="155" sheetId="4" r:id="rId4"/>
-    <sheet name="215" sheetId="7" r:id="rId5"/>
-    <sheet name="224" sheetId="8" r:id="rId6"/>
-    <sheet name="225" sheetId="5" r:id="rId7"/>
-    <sheet name="295" sheetId="9" r:id="rId8"/>
-    <sheet name="455" sheetId="10" r:id="rId9"/>
+    <sheet name="problem" sheetId="1" r:id="rId1"/>
+    <sheet name="155" sheetId="4" r:id="rId2"/>
+    <sheet name="215" sheetId="7" r:id="rId3"/>
+    <sheet name="224" sheetId="8" r:id="rId4"/>
+    <sheet name="225" sheetId="5" r:id="rId5"/>
+    <sheet name="295" sheetId="9" r:id="rId6"/>
+    <sheet name="376" sheetId="12" r:id="rId7"/>
+    <sheet name="455" sheetId="10" r:id="rId8"/>
+    <sheet name="402" sheetId="11" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,18 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>225. Implement Stack using Queues</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/implement-stack-using-queues/</t>
-  </si>
-  <si>
-    <t>approch#1</t>
-  </si>
-  <si>
-    <t>approch#2</t>
   </si>
   <si>
     <t>(Two Queues, push - O(n)O(n), pop O(1)O(1) )</t>
@@ -731,9 +726,6 @@
     }
 }</t>
     </r>
-  </si>
-  <si>
-    <t>默认小堆</t>
   </si>
   <si>
     <t>224. Basic Calculator</t>
@@ -1007,13 +999,6 @@
     </r>
   </si>
   <si>
-    <t>1                     注释掉这句话 //   state = State.NUM; 
-因为下个字符有可能是 （ ，仍然是OPT状态， 除非是0 -9才切到NUM状态
-2. enum 的变量声明需要加枚举类型State Switch中不需要。
-3. Stack 大小用size()
-4. char 的装箱类型为Character， 而不是Char</t>
-  </si>
-  <si>
     <t>分治</t>
   </si>
   <si>
@@ -1604,14 +1589,373 @@
     </r>
   </si>
   <si>
-    <t>java 写法好于 C++</t>
+    <t>402. Remove K Digits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-k-digits/</t>
+  </si>
+  <si>
+    <t>(One Stack)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        // String result = new String();
+        // for(Character c: s) {
+        //     result = result  + String.valueOf(c);
+        // }</t>
+  </si>
+  <si>
+    <t>1. 此部分效率和上边相差50%</t>
+  </si>
+  <si>
+    <r>
+      <t>class Solution {
+    public String removeKdigits(String num, int k) {
+        ArrayList&lt;Character&gt; s = new ArrayList&lt;Character&gt;();
+        Character cur;
+        for (int i = 0; i &lt; num.length(); i++) {
+            cur = num.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>charAt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(i);
+            while (s.size() != 0 &amp;&amp; s.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(s.size() - 1) &gt; cur &amp;&amp; k &gt; 0) {
+                s.remove(s.size() - 1);
+                k--;
+            }
+            if (s.size() == 0 &amp;&amp; cur == '0') {
+                //do nothing;
+            } else {
+                s.add(num.charAt(i));
+            }
+        }
+        while (k &gt; 0 &amp;&amp; s.size() != 0) {
+            s.remove(s.size() - 1);
+            k--;
+        }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        StringBuilder sb = new StringBuilder();
+        for (Character c : s) {
+            sb.append(c);
+        }
+        String result = sb.toString();
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        // String result = new String();
+        // for(Character c: s) {
+        //     result = result  + String.valueOf(c);
+        // }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        if (result.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>() == 0) return "0";
+        return result;
+    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. String::charAt ()
+2. String::length()
+3. ArrayList  a a[*] 不行， 要a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(index)
+4. char append to String
+ result = result  + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>String.valueOf(c);</t>
+    </r>
+  </si>
+  <si>
+    <t>默认小堆，自然顺序， 和C++默认不同</t>
+  </si>
+  <si>
+    <t>1 . 注释掉这句话 //   state = State.NUM; 
+因为下个字符有可能是 （ ，仍然是OPT状态， 除非是0 -9才切到NUM状态
+2. enum 的变量声明需要加枚举类型State Switch中不需要。
+3. Stack 大小用size()
+4. char 的装箱类型为Character， 而不是Char</t>
+  </si>
+  <si>
+    <t>java 写法好于 C++
+命名清晰</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class Solution {
+public:
+	string removeKdigits(string num, int k) {
+		vector&lt;char&gt; s;
+		string result;
+		char cur;
+		for (int i = 0; i &lt; num.length(); i++) {
+			cur = num[i];
+			while (s.size() &gt; 0 &amp;&amp; s.back() &gt; cur &amp;&amp; k-- &gt; 0) s.pop_back();
+			if (!s.empty() || cur != '0') </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s.push_back(cur);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+		}
+		while (!s.empty() &amp;&amp; k-- &gt; 0) s.pop_back();
+		for (char c : s) result += c;
+		if (result.empty()) return "0";
+		return result;
+	}
+};</t>
+    </r>
+  </si>
+  <si>
+    <t>注意笔误s.push_back(cur); 非 num.push_back(cur)</t>
+  </si>
+  <si>
+    <t>approach#1</t>
+  </si>
+  <si>
+    <t>approach#2</t>
+  </si>
+  <si>
+    <t>class Solution {
+private:
+	enum STATE {
+		BEGIN,
+		UP,
+		DOWN
+	};
+public:
+	int wiggleMaxLength(vector&lt;int&gt;&amp; nums) {
+		int size = nums.size();
+		if (size &lt; 2) return size;
+		STATE state = BEGIN;
+		int count = 1;
+		for (int i = 1; i &lt; nums.size(); i++) {
+			if (nums[i] == nums[i - 1]) continue;
+			switch (state) {
+			case BEGIN:
+				nums[i] &gt; nums[i - 1] ? state = UP : state = DOWN;
+				count++;
+				break;
+			case UP:
+				if (nums[i] &lt; nums[i - 1]) {
+					state = DOWN;
+					count++;
+				}
+				break;
+			case DOWN:
+				if (nums[i] &gt; nums[i - 1]) {
+					state = UP;
+					count++;
+				}
+				break;
+			}
+		}
+		return count;
+	}
+};</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class Solution {
+    private enum STATE {
+        BEGIN,
+        UP,
+        DOWN,
+    }
+    public int wiggleMaxLength(int[] nums) {
+        int count = 1;
+        STATE state = STATE.BEGIN;
+        if (nums.length &lt; 2) return nums.length;
+        for (int i = 1; i &lt; nums.length; i++) {
+            if (nums[i] == nums[i - 1]) continue;
+            switch (state) {
+                case BEGIN:
+                    if (nums[i] &gt; nums[i - 1]) state = STATE.UP;
+                    else state = STATE.DOWN;
+           </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">         // (nums[i] &gt; nums[i-1] ) ? state = STATE.UP : state = STATE.DOWN;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                    count++;
+                    break;
+                case UP:
+                    if (nums[i] &lt; nums[i - 1]) {
+                        state = STATE.DOWN;
+                        count++;
+                    }
+                    break;
+                case DOWN:
+                    if (nums[i] &gt; nums[i - 1]) {
+                        state = STATE.UP;
+                        count++;
+                    }
+                    break;
+            }
+        }
+        return count;
+    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         1. compiler error：           // (nums[i] &gt; nums[i-1] ) ? state = STATE.UP : state = STATE.DOWN;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 性能</t>
+  </si>
+  <si>
+    <t>编译错误</t>
+  </si>
+  <si>
+    <t>Stringbuilder 性能</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1708,6 +2052,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1751,7 +2101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1802,6 +2152,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1825,15 +2176,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>446886</xdr:colOff>
+      <xdr:colOff>627861</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1314286</xdr:rowOff>
+      <xdr:rowOff>1542886</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1856,7 +2207,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13944600" y="657225"/>
+          <a:off x="14125575" y="885825"/>
           <a:ext cx="6314286" cy="1314286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1869,15 +2220,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>532600</xdr:colOff>
+      <xdr:colOff>589750</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1352381</xdr:rowOff>
+      <xdr:rowOff>1504781</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1900,7 +2251,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13944600" y="5857875"/>
+          <a:off x="14001750" y="6010275"/>
           <a:ext cx="6400000" cy="1352381"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1963,6 +2314,55 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1162050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5010150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3581098</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DA79343-B7DB-42B3-9300-38EF2CCB8CBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8772525" y="1828800"/>
+          <a:ext cx="4505325" cy="2419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2099,7 +2499,188 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6753225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>666750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>46751</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4914369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794FB786-B33D-444C-A088-83DFE2107C65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16163925" y="6486525"/>
+          <a:ext cx="6990476" cy="4247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>6753225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>637313</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4752434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C50ABDF-9E98-42F1-87DB-85555F279D41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16163925" y="1047750"/>
+          <a:ext cx="6895238" cy="4323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1238249</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3162155</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4466362</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4914432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B064084-996A-48F8-AADA-5F5009A26666}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10648949" y="3781280"/>
+          <a:ext cx="3228113" cy="1752277"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>355746</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5095875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3495174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2876F427-BBC0-43B1-9A43-8340CEB1BCA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9972675" y="974871"/>
+          <a:ext cx="4533900" cy="3139428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2181,6 +2762,143 @@
         <a:xfrm>
           <a:off x="13906500" y="619125"/>
           <a:ext cx="4752134" cy="3506887"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>419101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>189750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3429001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FFEE4D-35BA-42CA-9255-40F28465CD54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14011275" y="1238251"/>
+          <a:ext cx="6000000" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>5086350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>818438</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>37576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAD10724-3AEC-4AA9-B51A-4FE1570CD20F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14106525" y="5905500"/>
+          <a:ext cx="5695238" cy="2552176"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>208806</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4066667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB260BE-58E5-4DAB-9394-A85EC0AA0573}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14077950" y="619125"/>
+          <a:ext cx="5952381" cy="4066667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2455,36 +3173,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>376</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>402</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="I21:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2494,7 +3234,7 @@
   <sheetData>
     <row r="21" spans="9:12">
       <c r="I21" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J21" s="7">
         <v>7</v>
@@ -2508,29 +3248,29 @@
     </row>
     <row r="22" spans="9:12">
       <c r="I22" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L22" s="7"/>
     </row>
     <row r="23" spans="9:12">
       <c r="I23" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="9:12">
       <c r="I26" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J26" s="8">
         <v>7</v>
@@ -2544,23 +3284,23 @@
     </row>
     <row r="27" spans="9:12">
       <c r="I27" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L27" s="7"/>
     </row>
     <row r="28" spans="9:12">
       <c r="I28" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L28" s="7"/>
     </row>
@@ -2569,12 +3309,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:E5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2586,19 +3326,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
       <c r="A1" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
       <c r="D1" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2607,10 +3347,10 @@
     <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" s="10" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -2619,26 +3359,26 @@
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.5">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2651,13 +3391,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4BB247-CC2B-46B0-988C-6416FE65FF1C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2670,7 +3411,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
@@ -2680,7 +3421,7 @@
     <row r="2" spans="1:6">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2689,10 +3430,10 @@
     <row r="3" spans="1:6">
       <c r="A3" s="11"/>
       <c r="B3" s="10" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -2701,35 +3442,35 @@
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="236.25">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -2738,29 +3479,29 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="409.5">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2770,12 +3511,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25713CA-613E-4C2D-A4B0-DC15A8BF32D4}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2787,7 +3528,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
@@ -2797,7 +3538,7 @@
     <row r="2" spans="1:5">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2806,10 +3547,10 @@
     <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" s="10" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -2818,39 +3559,40 @@
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.5">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2872,75 +3614,75 @@
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.5">
       <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.5">
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
         <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="409.5">
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="409.5">
       <c r="C8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="409.5">
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="409.5">
       <c r="C10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2948,12 +3690,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B18D55-11BE-4A9E-9686-DE2BF23140D6}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2965,7 +3707,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="11"/>
@@ -2975,7 +3717,7 @@
     <row r="2" spans="1:5">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2984,10 +3726,10 @@
     <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" s="10" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -2996,20 +3738,20 @@
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="2"/>
@@ -3017,10 +3759,10 @@
     <row r="6" spans="1:5">
       <c r="A6" s="11"/>
       <c r="B6" s="10" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -3029,10 +3771,10 @@
       <c r="A7" s="11"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E7" s="11"/>
     </row>
@@ -3040,13 +3782,13 @@
       <c r="A8" s="11"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3067,11 +3809,195 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE93C81B-018F-4E71-BFDC-586ABA93D637}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="89.875" customWidth="1"/>
+    <col min="5" max="5" width="89.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25">
+      <c r="A1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11"/>
+      <c r="B2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="11"/>
+      <c r="B3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="409.5">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="409.5">
+      <c r="A5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="3"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="3"/>
+      <c r="D10" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EFBECC34-3DCD-42E4-BAE5-D562BECE595E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0B7C73-9823-4163-88A2-1E29EBBE1584}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="11" style="3"/>
+    <col min="4" max="4" width="75.5" customWidth="1"/>
+    <col min="5" max="5" width="74.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25">
+      <c r="A1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11"/>
+      <c r="B2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="11"/>
+      <c r="B3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" ht="299.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="204.75">
+      <c r="A5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{95CDEE9F-7C25-430B-B925-18879B4C1B79}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9653F58-4956-4421-9009-E00391D6334C}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3083,7 +4009,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="10"/>
@@ -3103,41 +4029,51 @@
     <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" s="10" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="299.25">
+    <row r="4" spans="1:5" ht="346.5">
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="204.75">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5">
       <c r="A5" s="11"/>
       <c r="B5" s="10"/>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="78.75">
+      <c r="D6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{95CDEE9F-7C25-430B-B925-18879B4C1B79}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{CD97D57C-8C55-4F1C-98E5-8BCA52DED238}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>

</xml_diff>